<commit_message>
removed a trash file
</commit_message>
<xml_diff>
--- a/doc/specifiche.xlsx
+++ b/doc/specifiche.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,18 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="183">
   <si>
     <t xml:space="preserve">NOME FICO PLS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">by:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">io</t>
   </si>
   <si>
     <t xml:space="preserve">Versione 0.1</t>
@@ -825,9 +816,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>464760</xdr:colOff>
+      <xdr:colOff>464400</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -841,7 +832,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7959240" y="726840"/>
-          <a:ext cx="7876080" cy="5535720"/>
+          <a:ext cx="7887240" cy="5535360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -867,9 +858,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>178560</xdr:colOff>
+      <xdr:colOff>178200</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -882,8 +873,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9545760" y="956520"/>
-          <a:ext cx="7808040" cy="5745600"/>
+          <a:off x="9559800" y="956520"/>
+          <a:ext cx="7820280" cy="5745240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -909,9 +900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>198360</xdr:colOff>
+      <xdr:colOff>198000</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -924,8 +915,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9481680" y="754920"/>
-          <a:ext cx="7865280" cy="5086080"/>
+          <a:off x="9495720" y="754920"/>
+          <a:ext cx="7877520" cy="5085720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -948,10 +939,10 @@
   <dimension ref="B6:H22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
@@ -992,45 +983,39 @@
       <c r="H9" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C13" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="C13" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1054,243 +1039,243 @@
   </sheetPr>
   <dimension ref="A2:M76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="113.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M2" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1312,11 +1297,11 @@
   </sheetPr>
   <dimension ref="A2:S64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="16.53"/>
@@ -1326,12 +1311,12 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="4"/>
@@ -1340,16 +1325,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1357,15 +1342,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M6" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1391,42 +1377,43 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="P9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="P11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E12" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G13" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
       <c r="B15" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1450,71 +1437,72 @@
       <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2" t="s">
-        <v>72</v>
+      <c r="A17" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P18" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2" t="s">
-        <v>77</v>
+      <c r="A20" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P21" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M23" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="P21" s="4"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="P23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P24" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7"/>
       <c r="B28" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1540,46 +1528,46 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M30" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="P30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P31" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M33" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="P33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P34" s="4"/>
     </row>
@@ -1588,22 +1576,22 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M36" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="P36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D37" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P37" s="4"/>
     </row>
@@ -1611,8 +1599,9 @@
       <c r="M38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7"/>
       <c r="B39" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1637,25 +1626,25 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="P41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P42" s="5"/>
     </row>
@@ -1664,25 +1653,26 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="P44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I45" s="2"/>
       <c r="J45" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7"/>
       <c r="B46" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -1701,11 +1691,12 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G47" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P47" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -1726,8 +1717,9 @@
       <c r="S49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7"/>
       <c r="B50" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -1749,96 +1741,96 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="I51" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M51" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="O51" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="O51" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="Q51" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D54" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D61" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1860,263 +1852,263 @@
   <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H61" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2142,125 +2134,125 @@
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2285,51 +2277,51 @@
       <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M4" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2355,41 +2347,41 @@
       <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2414,26 +2406,26 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>